<commit_message>
Updated time sheets and some minor changes to report
</commit_message>
<xml_diff>
--- a/man/completed sheets/2016-01-25/Ben_Dudley_Timesheet_25.01.16.xlsx
+++ b/man/completed sheets/2016-01-25/Ben_Dudley_Timesheet_25.01.16.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\Ben Dudley Timesheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\Github\cs221\man\completed sheets\2016-01-25\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -107,13 +107,13 @@
     <t>Attempted to rearrange code so that users and tasks would be saved</t>
   </si>
   <si>
-    <t>Total hours accounted this week: 13:30</t>
+    <t>Total hours accounted this week: 29.30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
@@ -486,21 +486,21 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
-    <col min="8" max="8" width="36.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" customWidth="1"/>
+    <col min="8" max="8" width="36.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -524,7 +524,7 @@
       </c>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -548,7 +548,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="48" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="47.4" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>18</v>
       </c>
@@ -565,12 +565,12 @@
         <v>42398</v>
       </c>
       <c r="F3" s="10">
-        <v>6.25E-2</v>
+        <v>0.1875</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8" ht="63.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="63" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>22</v>
       </c>
@@ -587,14 +587,14 @@
         <v>42398</v>
       </c>
       <c r="F4" s="10">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="48" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="47.4" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>20</v>
       </c>
@@ -616,7 +616,7 @@
       <c r="G5" s="7"/>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="1:8" ht="48" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="47.4" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>20</v>
       </c>
@@ -640,7 +640,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>20</v>
       </c>

</xml_diff>